<commit_message>
implement premium learn page
</commit_message>
<xml_diff>
--- a/front-end/src/assets/files/Template.xlsx
+++ b/front-end/src/assets/files/Template.xlsx
@@ -1,41 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SmartQuizProject\front-end\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0064903-B93B-416B-ACB2-7D9B7C9EC8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273BD39A-26C0-4F55-8DC4-932225B083F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B2AD69D-3BEE-49DB-B933-D3DDEC81D611}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="4">
   <si>
-    <t>Question Template</t>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -386,21 +387,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C8161A-4F46-4DB9-B60D-7D8681C5F0FB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 O2:O1048576 E2:E1048576 G2:G1048576 I2:I1048576 K2:K1048576 M2:M1048576 Q2:Q1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$Z$2:$Z$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>